<commit_message>
Added support to user defined drug naming
Changed example.xlsx to support variable drug naming
</commit_message>
<xml_diff>
--- a/example.xlsx
+++ b/example.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chiragbhat/PycharmProjects/Resiquimod Calculator/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF0E67D9-7858-CB49-8E02-F562254D4520}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CFF3944A-038E-9743-8DD5-52BE3D785979}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="740" windowWidth="29040" windowHeight="15720" xr2:uid="{D7523CA5-ED54-42B2-9640-CB2F5E95C523}"/>
   </bookViews>
@@ -89,15 +89,6 @@
     <t>Time</t>
   </si>
   <si>
-    <t>R848 SWNTs 1</t>
-  </si>
-  <si>
-    <t>R848 SWNTs 2</t>
-  </si>
-  <si>
-    <t>R848 SWNTs 3</t>
-  </si>
-  <si>
     <t>SWNT Control 1</t>
   </si>
   <si>
@@ -128,9 +119,6 @@
     <t>Absorption 808 nm</t>
   </si>
   <si>
-    <t>R8484 SWNTs 3</t>
-  </si>
-  <si>
     <t>SWNTs Control 1</t>
   </si>
   <si>
@@ -144,13 +132,25 @@
   </si>
   <si>
     <t>All of the headers you see must remain exactly the same.</t>
+  </si>
+  <si>
+    <t>Required (string)</t>
+  </si>
+  <si>
+    <t>[INSERT DRUG NAME] SWNTs 1</t>
+  </si>
+  <si>
+    <t>[INSERT DRUG NAME] SWNTs 2</t>
+  </si>
+  <si>
+    <t>[INSERT DRUG NAME] SWNTs 3</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -192,6 +192,12 @@
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -576,7 +582,7 @@
   <dimension ref="A1:P47"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="E16" sqref="E16:G16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -603,7 +609,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>12</v>
+        <v>32</v>
       </c>
       <c r="D1" s="3" t="s">
         <v>15</v>
@@ -632,40 +638,40 @@
         <v>16</v>
       </c>
       <c r="E2" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="F2" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="G2" s="5" t="s">
+        <v>35</v>
+      </c>
+      <c r="H2" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="F2" s="3" t="s">
+      <c r="I2" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="G2" s="6" t="s">
+      <c r="J2" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="H2" s="3" t="s">
+      <c r="K2" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="I2" s="3" t="s">
+      <c r="L2" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="J2" s="3" t="s">
+      <c r="M2" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="K2" s="3" t="s">
+      <c r="N2" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="L2" s="3" t="s">
+      <c r="O2" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="M2" s="3" t="s">
+      <c r="P2" s="1" t="s">
         <v>25</v>
-      </c>
-      <c r="N2" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="O2" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="P2" s="1" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="3" spans="1:16" ht="16" x14ac:dyDescent="0.2">
@@ -1181,7 +1187,7 @@
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.2">
       <c r="B14" s="2" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="D14" s="2"/>
       <c r="E14" s="2"/>
@@ -1194,7 +1200,7 @@
     </row>
     <row r="15" spans="1:16" ht="16" x14ac:dyDescent="0.2">
       <c r="D15" s="6" t="s">
-        <v>29</v>
+        <v>26</v>
       </c>
       <c r="E15" s="4"/>
       <c r="F15" s="4"/>
@@ -1211,46 +1217,46 @@
     </row>
     <row r="16" spans="1:16" ht="16" x14ac:dyDescent="0.2">
       <c r="B16" s="8" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="D16" s="6" t="s">
         <v>16</v>
       </c>
-      <c r="E16" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="F16" s="6" t="s">
-        <v>18</v>
-      </c>
-      <c r="G16" s="6" t="s">
-        <v>30</v>
+      <c r="E16" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="F16" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="G16" s="5" t="s">
+        <v>35</v>
       </c>
       <c r="H16" s="6" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="I16" s="6" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="J16" s="6" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="K16" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="L16" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="M16" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="N16" s="1" t="s">
         <v>23</v>
       </c>
-      <c r="L16" s="6" t="s">
+      <c r="O16" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="M16" s="6" t="s">
+      <c r="P16" s="1" t="s">
         <v>25</v>
-      </c>
-      <c r="N16" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="O16" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="P16" s="1" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="17" spans="4:16" x14ac:dyDescent="0.2">
@@ -1813,6 +1819,7 @@
       <c r="P47" s="2"/>
     </row>
   </sheetData>
+  <phoneticPr fontId="6" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>